<commit_message>
internal consistency, per-item violin plots, bugfixes
</commit_message>
<xml_diff>
--- a/information/2025-10-28_Scoring.xlsx
+++ b/information/2025-10-28_Scoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207F9DDE-B62D-4ADF-AC27-0508CA6A81FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B990BAF-9F20-4B00-AAC3-17E89B03B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="5820" windowWidth="19185" windowHeight="10065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>